<commit_message>
Committing SPPCase2 pagination work
</commit_message>
<xml_diff>
--- a/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Suite StatutoryMaternityPay201718.xlsx
+++ b/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Suite StatutoryMaternityPay201718.xlsx
@@ -4,29 +4,29 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="396" yWindow="36" windowWidth="15168" windowHeight="5400" activeTab="3"/>
+    <workbookView activeTab="3" windowHeight="5400" windowWidth="15168" xWindow="396" yWindow="36"/>
   </bookViews>
   <sheets>
-    <sheet name="first" sheetId="1" r:id="rId1"/>
-    <sheet name="ResetData" sheetId="15" r:id="rId2"/>
-    <sheet name="CreateFemaleEmployee" sheetId="2" r:id="rId3"/>
-    <sheet name="UpdateTaxCodeAndAnnualSalary" sheetId="6" r:id="rId4"/>
-    <sheet name="SmallEmployerRelief" sheetId="3" r:id="rId5"/>
-    <sheet name="ProcessPayrollForAprilMonthSMP" sheetId="7" r:id="rId6"/>
-    <sheet name="ProcessPayrollForMayMonthSMP" sheetId="8" r:id="rId7"/>
-    <sheet name="ProcessPayrollForJuneMonthSMP" sheetId="9" r:id="rId8"/>
-    <sheet name="CreateLeaveRequest" sheetId="10" r:id="rId9"/>
-    <sheet name="AverageWeeklyEarningsTestReport" sheetId="14" r:id="rId10"/>
-    <sheet name="ProcessPayrollForNovMonthSMP" sheetId="11" r:id="rId11"/>
-    <sheet name="ProcessPayrollForDecMonthSMP" sheetId="12" r:id="rId12"/>
-    <sheet name="ProcessPayrollForJan2016MontSMP" sheetId="13" r:id="rId13"/>
+    <sheet name="first" r:id="rId1" sheetId="1"/>
+    <sheet name="ResetData" r:id="rId2" sheetId="15"/>
+    <sheet name="CreateFemaleEmployee" r:id="rId3" sheetId="2"/>
+    <sheet name="UpdateTaxCodeAndAnnualSalary" r:id="rId4" sheetId="6"/>
+    <sheet name="SmallEmployerRelief" r:id="rId5" sheetId="3"/>
+    <sheet name="ProcessPayrollForAprilMonthSMP" r:id="rId6" sheetId="7"/>
+    <sheet name="ProcessPayrollForMayMonthSMP" r:id="rId7" sheetId="8"/>
+    <sheet name="ProcessPayrollForJuneMonthSMP" r:id="rId8" sheetId="9"/>
+    <sheet name="CreateLeaveRequest" r:id="rId9" sheetId="10"/>
+    <sheet name="AverageWeeklyEarningsTestReport" r:id="rId10" sheetId="14"/>
+    <sheet name="ProcessPayrollForNovMonthSMP" r:id="rId11" sheetId="11"/>
+    <sheet name="ProcessPayrollForDecMonthSMP" r:id="rId12" sheetId="12"/>
+    <sheet name="ProcessPayrollForJan2016MontSMP" r:id="rId13" sheetId="13"/>
   </sheets>
   <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="188">
   <si>
     <t>TC</t>
   </si>
@@ -596,6 +596,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -660,64 +661,64 @@
     </border>
   </borders>
   <cellStyleXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="23">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf applyFill="1" borderId="0" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyProtection="1" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="2">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0"/>
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
     <cellStyle name="Normal 2" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -734,10 +735,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -895,7 +896,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -904,13 +905,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -920,7 +921,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -929,7 +930,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -938,7 +939,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -948,12 +949,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -984,7 +985,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -1003,7 +1004,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -1015,7 +1016,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1024,13 +1025,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.44140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="44.33203125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="17.33203125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="32.44140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="44.33203125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="17.33203125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.44140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1044,7 +1045,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>99</v>
       </c>
@@ -1058,7 +1059,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>159</v>
       </c>
@@ -1072,7 +1073,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>101</v>
       </c>
@@ -1083,7 +1084,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>106</v>
       </c>
@@ -1097,7 +1098,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>114</v>
       </c>
@@ -1111,7 +1112,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>117</v>
       </c>
@@ -1128,7 +1129,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>126</v>
       </c>
@@ -1142,7 +1143,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>120</v>
       </c>
@@ -1156,7 +1157,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>128</v>
       </c>
@@ -1311,12 +1312,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
@@ -1325,20 +1326,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="36.33203125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="31" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.33203125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.88671875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.88671875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="30.33203125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="36" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="39.33203125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.33203125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="14.6640625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="23.44140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="36.33203125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="31.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="16.33203125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.88671875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.88671875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="30.33203125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="36.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="39.33203125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.33203125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="14.6640625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="23.44140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>146</v>
       </c>
@@ -1382,7 +1383,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="20" customFormat="1" ht="84.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="84.6" r="2" s="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="22" t="s">
         <v>185</v>
       </c>
@@ -1420,14 +1421,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
@@ -1436,20 +1437,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="28.6640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="20" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.6640625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="18.44140625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="28.88671875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="32.44140625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="39.6640625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.33203125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="15.6640625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="22.109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="35.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="28.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="12.6640625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="18.44140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="28.88671875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="32.44140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="39.6640625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.33203125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="15.6640625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="22.109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>146</v>
       </c>
@@ -1493,7 +1494,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="20" customFormat="1" ht="73.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="73.95" r="2" s="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="22" t="s">
         <v>185</v>
       </c>
@@ -1533,14 +1534,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="F1" workbookViewId="0">
@@ -1549,18 +1550,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="37" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="35.6640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="22.33203125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.44140625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="31.6640625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="32.44140625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="37.33203125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12.44140625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="28.44140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="37.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="35.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="22.33203125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.44140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="31.6640625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="32.44140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="37.33203125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="12.44140625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="28.44140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>146</v>
       </c>
@@ -1604,7 +1605,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="20" customFormat="1" ht="58.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="58.95" r="2" s="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="22" t="s">
         <v>185</v>
       </c>
@@ -1644,15 +1645,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId2" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1661,20 +1662,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.6640625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="35.44140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.6640625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.6640625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.6640625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="30.109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="35.109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="34" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.44140625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="14.109375" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="22.33203125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="35.6640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="35.44140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="16.6640625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="12.6640625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.6640625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="30.109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="35.109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="34.0" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.44140625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="14.109375" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="22.33203125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>146</v>
       </c>
@@ -1718,7 +1719,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="20" customFormat="1" ht="93.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="93.6" r="2" s="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="22" t="s">
         <v>185</v>
       </c>
@@ -1758,14 +1759,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1774,11 +1775,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="17.44140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="35.0" collapsed="true"/>
+    <col min="2" max="3" customWidth="true" width="17.44140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>98</v>
       </c>
@@ -1798,7 +1799,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="21.6" r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>104</v>
       </c>
@@ -1813,13 +1814,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BK2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1828,15 +1829,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.33203125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="27.5546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="27.6640625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="24.88671875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="19.6640625" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="24.6640625" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="15.44140625" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="22.33203125" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="25" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="19.33203125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="27.5546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="27.6640625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="24.88671875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="19.6640625" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" width="24.6640625" collapsed="true"/>
+    <col min="37" max="37" customWidth="true" width="15.44140625" collapsed="true"/>
+    <col min="38" max="38" customWidth="true" width="22.33203125" collapsed="true"/>
+    <col min="39" max="39" customWidth="true" width="25.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:63" x14ac:dyDescent="0.25">
@@ -2217,15 +2218,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="D2" r:id="rId2"/>
+    <hyperlink r:id="rId1" ref="C2"/>
+    <hyperlink r:id="rId2" ref="D2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -2234,12 +2235,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="43.6640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="17.109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="24.88671875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="43.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="17.109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="24.88671875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>98</v>
       </c>
@@ -2265,7 +2266,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="21.6" r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>104</v>
       </c>
@@ -2286,12 +2287,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2300,11 +2301,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="48.33203125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="22.6640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="48.33203125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="22.6640625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>98</v>
       </c>
@@ -2321,7 +2322,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="17.399999999999999" r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>104</v>
       </c>
@@ -2333,13 +2334,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
@@ -2348,21 +2349,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="53.5546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="36.5546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.33203125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.44140625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="31.88671875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="28.6640625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="40.33203125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.109375" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12.109375" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="23.5546875" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="10.88671875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="53.5546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="36.5546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="15.109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.33203125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.44140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="31.88671875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="28.6640625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="40.33203125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.109375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="12.109375" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="23.5546875" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="10.88671875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>146</v>
       </c>
@@ -2406,7 +2407,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="20" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="60" r="2" s="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="22" t="s">
         <v>185</v>
       </c>
@@ -2446,15 +2447,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId2" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
@@ -2463,19 +2464,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="42.5546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="38.44140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.33203125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.33203125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.5546875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="24.33203125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="25.5546875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="34.33203125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="10.6640625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="16.88671875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="42.5546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="38.44140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="14.33203125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.33203125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="16.5546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="24.33203125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="25.5546875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="34.33203125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="10.6640625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="16.88671875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>146</v>
       </c>
@@ -2519,7 +2520,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="20" customFormat="1" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="69.599999999999994" r="2" s="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="22" t="s">
         <v>185</v>
       </c>
@@ -2559,14 +2560,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
@@ -2575,20 +2576,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="37.6640625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="28.44140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="17.5546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.33203125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.44140625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="33.6640625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="22.44140625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="38.5546875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12.33203125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="22.88671875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="37.6640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="28.44140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="17.5546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="13.33203125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.44140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="33.6640625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="22.44140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="38.5546875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="12.33203125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="22.88671875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>146</v>
       </c>
@@ -2632,7 +2633,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="20" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="60" r="2" s="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="22" t="s">
         <v>185</v>
       </c>
@@ -2672,14 +2673,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2688,13 +2689,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="37.33203125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.5546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.6640625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.88671875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="16.33203125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="13.6640625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="36.44140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="37.33203125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="15.5546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="12.6640625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.88671875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="16.33203125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="13.6640625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="36.44140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -2771,7 +2772,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>